<commit_message>
specify plane to all patterns
</commit_message>
<xml_diff>
--- a/pyCGM2/Settings/jointPatterns/Nieuwenhuys2017.xlsx
+++ b/pyCGM2/Settings/jointPatterns/Nieuwenhuys2017.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HLS501\Documents\Programming\API\pyCGM2\pyCGM2\pyCGM2\Settings\jointPatterns\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9C050C-890F-4192-AC14-EC72615AF08B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="4" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2894" uniqueCount="328">
   <si>
     <t>Plan</t>
   </si>
@@ -1113,8 +1119,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1181,8 +1187,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1272,6 +1285,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -1354,12 +1385,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1642,12 +1676,6 @@
     <xf numFmtId="49" fontId="0" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1684,8 +1712,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="9" fillId="16" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="6">
+    <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="5" builtinId="32"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1695,6 +1735,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1743,7 +1786,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1776,9 +1819,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1811,6 +1871,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1986,10 +2063,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="C22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
@@ -4257,11 +4334,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80:A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4302,7 +4379,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="112" t="s">
         <v>84</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -4321,6 +4398,9 @@
       <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B3" s="22" t="s">
         <v>10</v>
       </c>
@@ -4335,6 +4415,9 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B4" s="22" t="s">
         <v>10</v>
       </c>
@@ -4349,6 +4432,9 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B5" s="22" t="s">
         <v>10</v>
       </c>
@@ -4363,6 +4449,9 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B6" s="22" t="s">
         <v>10</v>
       </c>
@@ -4377,7 +4466,9 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
+      <c r="A7" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B7" s="23" t="s">
         <v>10</v>
       </c>
@@ -4395,6 +4486,9 @@
       <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B8" s="22" t="s">
         <v>85</v>
       </c>
@@ -4413,6 +4507,9 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B9" s="22" t="s">
         <v>85</v>
       </c>
@@ -4430,26 +4527,31 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="102"/>
-      <c r="B10" s="102" t="s">
+      <c r="A10" s="112" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="100" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="105" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="102"/>
-      <c r="E10" s="102" t="s">
+      <c r="C10" s="103" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="100"/>
+      <c r="E10" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="102" t="s">
+      <c r="F10" s="100" t="s">
         <v>162</v>
       </c>
-      <c r="G10" s="102" t="s">
+      <c r="G10" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="102"/>
+      <c r="H10" s="100"/>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B11" s="22" t="s">
         <v>11</v>
       </c>
@@ -4471,6 +4573,9 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B12" s="22" t="s">
         <v>11</v>
       </c>
@@ -4488,6 +4593,9 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B13" s="22" t="s">
         <v>11</v>
       </c>
@@ -4505,6 +4613,9 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B14" s="22" t="s">
         <v>11</v>
       </c>
@@ -4525,6 +4636,9 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B15" s="22" t="s">
         <v>11</v>
       </c>
@@ -4545,6 +4659,9 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B16" s="22" t="s">
         <v>11</v>
       </c>
@@ -4565,27 +4682,33 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="106" t="s">
+      <c r="A17" s="112" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="104" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="107" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="108" t="s">
+      <c r="C17" s="105" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="106" t="s">
         <v>152</v>
       </c>
-      <c r="E17" s="108" t="s">
+      <c r="E17" s="106" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="108" t="s">
+      <c r="F17" s="106" t="s">
         <v>191</v>
       </c>
-      <c r="G17" s="106" t="s">
+      <c r="G17" s="104" t="s">
         <v>41</v>
       </c>
-      <c r="H17" s="106"/>
+      <c r="H17" s="104"/>
     </row>
     <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B18" s="22" t="s">
         <v>11</v>
       </c>
@@ -4605,6 +4728,9 @@
       <c r="H18" s="38"/>
     </row>
     <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B19" s="22" t="s">
         <v>11</v>
       </c>
@@ -4622,6 +4748,9 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B20" s="22" t="s">
         <v>11</v>
       </c>
@@ -4639,6 +4768,9 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B21" s="22" t="s">
         <v>11</v>
       </c>
@@ -4656,6 +4788,9 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B22" s="22" t="s">
         <v>11</v>
       </c>
@@ -4673,7 +4808,9 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23"/>
+      <c r="A23" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B23" s="23" t="s">
         <v>11</v>
       </c>
@@ -4690,9 +4827,12 @@
         <v>180</v>
       </c>
       <c r="G23" s="23"/>
-      <c r="H23" s="102"/>
+      <c r="H23" s="100"/>
     </row>
     <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B24" s="22" t="s">
         <v>94</v>
       </c>
@@ -4712,6 +4852,9 @@
       <c r="H24" s="38"/>
     </row>
     <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B25" s="22" t="s">
         <v>94</v>
       </c>
@@ -4732,6 +4875,9 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B26" s="22" t="s">
         <v>94</v>
       </c>
@@ -4752,6 +4898,9 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B27" s="22" t="s">
         <v>94</v>
       </c>
@@ -4772,27 +4921,33 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="106" t="s">
+      <c r="A28" s="112" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="104" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="107" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="108" t="s">
+      <c r="C28" s="105" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="106" t="s">
         <v>154</v>
       </c>
-      <c r="E28" s="108" t="s">
+      <c r="E28" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="F28" s="108" t="s">
+      <c r="F28" s="106" t="s">
         <v>195</v>
       </c>
-      <c r="G28" s="106" t="s">
+      <c r="G28" s="104" t="s">
         <v>58</v>
       </c>
-      <c r="H28" s="106"/>
+      <c r="H28" s="104"/>
     </row>
     <row r="29" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B29" s="22" t="s">
         <v>94</v>
       </c>
@@ -4810,6 +4965,9 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B30" s="22" t="s">
         <v>94</v>
       </c>
@@ -4830,6 +4988,9 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B31" s="22" t="s">
         <v>94</v>
       </c>
@@ -4850,7 +5011,9 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="70"/>
+      <c r="A32" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B32" s="70" t="s">
         <v>94</v>
       </c>
@@ -4872,7 +5035,7 @@
       <c r="H32" s="70"/>
     </row>
     <row r="33" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="101" t="s">
+      <c r="A33" s="113" t="s">
         <v>95</v>
       </c>
       <c r="B33" s="22" t="s">
@@ -4886,6 +5049,9 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="113" t="s">
+        <v>95</v>
+      </c>
       <c r="B34" s="22" t="s">
         <v>10</v>
       </c>
@@ -4897,6 +5063,9 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="113" t="s">
+        <v>95</v>
+      </c>
       <c r="B35" s="22" t="s">
         <v>10</v>
       </c>
@@ -4908,6 +5077,9 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="113" t="s">
+        <v>95</v>
+      </c>
       <c r="B36" s="22" t="s">
         <v>10</v>
       </c>
@@ -4919,10 +5091,13 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="113" t="s">
+        <v>95</v>
+      </c>
       <c r="B37" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="104" t="s">
+      <c r="C37" s="102" t="s">
         <v>92</v>
       </c>
       <c r="E37" s="69" t="s">
@@ -4933,10 +5108,13 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="113" t="s">
+        <v>95</v>
+      </c>
       <c r="B38" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C38" s="104" t="s">
+      <c r="C38" s="102" t="s">
         <v>92</v>
       </c>
       <c r="D38" s="51" t="s">
@@ -4950,10 +5128,13 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="113" t="s">
+        <v>95</v>
+      </c>
       <c r="B39" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="104" t="s">
+      <c r="C39" s="102" t="s">
         <v>92</v>
       </c>
       <c r="E39" s="66" t="s">
@@ -4964,7 +5145,9 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="70"/>
+      <c r="A40" s="113" t="s">
+        <v>95</v>
+      </c>
       <c r="B40" s="70" t="s">
         <v>85</v>
       </c>
@@ -4982,7 +5165,7 @@
       <c r="H40" s="70"/>
     </row>
     <row r="41" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="101" t="s">
+      <c r="A41" s="114" t="s">
         <v>230</v>
       </c>
       <c r="B41" s="22" t="s">
@@ -4998,6 +5181,9 @@
       <c r="H41" s="92"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="114" t="s">
+        <v>230</v>
+      </c>
       <c r="B42" s="22" t="s">
         <v>10</v>
       </c>
@@ -5011,6 +5197,9 @@
       <c r="H42" s="92"/>
     </row>
     <row r="43" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="114" t="s">
+        <v>230</v>
+      </c>
       <c r="B43" s="22" t="s">
         <v>10</v>
       </c>
@@ -5024,6 +5213,9 @@
       <c r="H43" s="92"/>
     </row>
     <row r="44" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="114" t="s">
+        <v>230</v>
+      </c>
       <c r="B44" s="22" t="s">
         <v>10</v>
       </c>
@@ -5037,6 +5229,9 @@
       <c r="H44" s="92"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="114" t="s">
+        <v>230</v>
+      </c>
       <c r="B45" s="22" t="s">
         <v>85</v>
       </c>
@@ -5053,6 +5248,9 @@
       <c r="H45" s="92"/>
     </row>
     <row r="46" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="114" t="s">
+        <v>230</v>
+      </c>
       <c r="B46" s="22" t="s">
         <v>85</v>
       </c>
@@ -5069,6 +5267,9 @@
       <c r="H46" s="92"/>
     </row>
     <row r="47" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="114" t="s">
+        <v>230</v>
+      </c>
       <c r="B47" s="22" t="s">
         <v>85</v>
       </c>
@@ -5085,6 +5286,9 @@
       <c r="H47" s="92"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="114" t="s">
+        <v>230</v>
+      </c>
       <c r="B48" s="22" t="s">
         <v>235</v>
       </c>
@@ -5104,6 +5308,9 @@
       <c r="H48" s="92"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="114" t="s">
+        <v>230</v>
+      </c>
       <c r="B49" s="22" t="s">
         <v>235</v>
       </c>
@@ -5124,7 +5331,9 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="70"/>
+      <c r="A50" s="114" t="s">
+        <v>230</v>
+      </c>
       <c r="B50" s="70" t="s">
         <v>235</v>
       </c>
@@ -5146,7 +5355,7 @@
       <c r="H50" s="70"/>
     </row>
     <row r="51" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="100" t="s">
+      <c r="A51" s="112" t="s">
         <v>84</v>
       </c>
       <c r="B51" s="22" t="s">
@@ -5167,6 +5376,9 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A52" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B52" s="22" t="s">
         <v>85</v>
       </c>
@@ -5184,6 +5396,9 @@
       </c>
     </row>
     <row r="53" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B53" s="22" t="s">
         <v>85</v>
       </c>
@@ -5201,6 +5416,9 @@
       </c>
     </row>
     <row r="54" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A54" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B54" s="22" t="s">
         <v>11</v>
       </c>
@@ -5222,6 +5440,9 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B55" s="22" t="s">
         <v>11</v>
       </c>
@@ -5239,6 +5460,9 @@
       </c>
     </row>
     <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B56" s="22" t="s">
         <v>11</v>
       </c>
@@ -5256,6 +5480,9 @@
       </c>
     </row>
     <row r="57" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A57" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B57" s="22" t="s">
         <v>11</v>
       </c>
@@ -5276,6 +5503,9 @@
       </c>
     </row>
     <row r="58" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B58" s="22" t="s">
         <v>11</v>
       </c>
@@ -5296,6 +5526,9 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A59" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B59" s="22" t="s">
         <v>11</v>
       </c>
@@ -5316,27 +5549,33 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B60" s="106" t="s">
+      <c r="A60" s="112" t="s">
+        <v>84</v>
+      </c>
+      <c r="B60" s="104" t="s">
         <v>11</v>
       </c>
-      <c r="C60" s="109" t="s">
+      <c r="C60" s="107" t="s">
         <v>225</v>
       </c>
-      <c r="D60" s="110" t="s">
+      <c r="D60" s="108" t="s">
         <v>152</v>
       </c>
-      <c r="E60" s="110" t="s">
+      <c r="E60" s="108" t="s">
         <v>40</v>
       </c>
-      <c r="F60" s="110" t="s">
+      <c r="F60" s="108" t="s">
         <v>300</v>
       </c>
-      <c r="G60" s="106" t="s">
+      <c r="G60" s="104" t="s">
         <v>41</v>
       </c>
-      <c r="H60" s="106"/>
+      <c r="H60" s="104"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B61" s="22" t="s">
         <v>11</v>
       </c>
@@ -5356,6 +5595,9 @@
       <c r="H61" s="38"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B62" s="22" t="s">
         <v>11</v>
       </c>
@@ -5373,6 +5615,9 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B63" s="22" t="s">
         <v>11</v>
       </c>
@@ -5390,6 +5635,9 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B64" s="22" t="s">
         <v>11</v>
       </c>
@@ -5407,6 +5655,9 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B65" s="22" t="s">
         <v>11</v>
       </c>
@@ -5424,11 +5675,13 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="23"/>
+      <c r="A66" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B66" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C66" s="103" t="s">
+      <c r="C66" s="101" t="s">
         <v>225</v>
       </c>
       <c r="D66" s="99" t="s">
@@ -5441,9 +5694,12 @@
         <v>306</v>
       </c>
       <c r="G66" s="23"/>
-      <c r="H66" s="102"/>
+      <c r="H66" s="100"/>
     </row>
     <row r="67" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A67" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B67" s="22" t="s">
         <v>94</v>
       </c>
@@ -5462,6 +5718,9 @@
       <c r="G67" s="38"/>
     </row>
     <row r="68" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A68" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B68" s="22" t="s">
         <v>94</v>
       </c>
@@ -5482,6 +5741,9 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A69" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B69" s="22" t="s">
         <v>94</v>
       </c>
@@ -5502,6 +5764,9 @@
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B70" s="22" t="s">
         <v>94</v>
       </c>
@@ -5522,27 +5787,33 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B71" s="106" t="s">
+      <c r="A71" s="112" t="s">
+        <v>84</v>
+      </c>
+      <c r="B71" s="104" t="s">
         <v>94</v>
       </c>
-      <c r="C71" s="109" t="s">
+      <c r="C71" s="107" t="s">
         <v>225</v>
       </c>
-      <c r="D71" s="110" t="s">
+      <c r="D71" s="108" t="s">
         <v>154</v>
       </c>
-      <c r="E71" s="110" t="s">
+      <c r="E71" s="108" t="s">
         <v>57</v>
       </c>
-      <c r="F71" s="110" t="s">
+      <c r="F71" s="108" t="s">
         <v>312</v>
       </c>
-      <c r="G71" s="106" t="s">
+      <c r="G71" s="104" t="s">
         <v>58</v>
       </c>
-      <c r="H71" s="106"/>
+      <c r="H71" s="104"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B72" s="22" t="s">
         <v>94</v>
       </c>
@@ -5560,6 +5831,9 @@
       </c>
     </row>
     <row r="73" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A73" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B73" s="22" t="s">
         <v>94</v>
       </c>
@@ -5580,6 +5854,9 @@
       </c>
     </row>
     <row r="74" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B74" s="22" t="s">
         <v>94</v>
       </c>
@@ -5600,7 +5877,9 @@
       </c>
     </row>
     <row r="75" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="70"/>
+      <c r="A75" s="112" t="s">
+        <v>84</v>
+      </c>
       <c r="B75" s="70" t="s">
         <v>94</v>
       </c>
@@ -5622,7 +5901,7 @@
       <c r="H75" s="70"/>
     </row>
     <row r="76" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="101" t="s">
+      <c r="A76" s="113" t="s">
         <v>95</v>
       </c>
       <c r="B76" s="22" t="s">
@@ -5639,6 +5918,9 @@
       </c>
     </row>
     <row r="77" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="113" t="s">
+        <v>95</v>
+      </c>
       <c r="B77" s="22" t="s">
         <v>85</v>
       </c>
@@ -5656,6 +5938,9 @@
       </c>
     </row>
     <row r="78" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A78" s="113" t="s">
+        <v>95</v>
+      </c>
       <c r="B78" s="22" t="s">
         <v>85</v>
       </c>
@@ -5670,7 +5955,9 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="70"/>
+      <c r="A79" s="113" t="s">
+        <v>95</v>
+      </c>
       <c r="B79" s="70" t="s">
         <v>85</v>
       </c>
@@ -5688,7 +5975,7 @@
       <c r="H79" s="70"/>
     </row>
     <row r="80" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="101" t="s">
+      <c r="A80" s="114" t="s">
         <v>230</v>
       </c>
       <c r="B80" s="22" t="s">
@@ -5705,6 +5992,9 @@
       </c>
     </row>
     <row r="81" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="114" t="s">
+        <v>230</v>
+      </c>
       <c r="B81" s="22" t="s">
         <v>85</v>
       </c>
@@ -5720,24 +6010,29 @@
       <c r="G81" s="64"/>
     </row>
     <row r="82" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="102"/>
-      <c r="B82" s="102" t="s">
+      <c r="A82" s="114" t="s">
+        <v>230</v>
+      </c>
+      <c r="B82" s="100" t="s">
         <v>85</v>
       </c>
-      <c r="C82" s="103" t="s">
+      <c r="C82" s="101" t="s">
         <v>225</v>
       </c>
-      <c r="D82" s="102"/>
-      <c r="E82" s="111" t="s">
+      <c r="D82" s="100"/>
+      <c r="E82" s="109" t="s">
         <v>234</v>
       </c>
-      <c r="F82" s="102" t="s">
+      <c r="F82" s="100" t="s">
         <v>322</v>
       </c>
-      <c r="G82" s="112"/>
-      <c r="H82" s="102"/>
+      <c r="G82" s="110"/>
+      <c r="H82" s="100"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A83" s="114" t="s">
+        <v>230</v>
+      </c>
       <c r="B83" s="22" t="s">
         <v>235</v>
       </c>
@@ -5756,6 +6051,9 @@
       <c r="G83" s="64"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A84" s="114" t="s">
+        <v>230</v>
+      </c>
       <c r="B84" s="22" t="s">
         <v>235</v>
       </c>
@@ -5776,7 +6074,9 @@
       </c>
     </row>
     <row r="85" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="70"/>
+      <c r="A85" s="114" t="s">
+        <v>230</v>
+      </c>
       <c r="B85" s="70" t="s">
         <v>235</v>
       </c>
@@ -5813,7 +6113,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView topLeftCell="A37" workbookViewId="0">
@@ -5931,10 +6231,10 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="113" t="s">
+      <c r="A12" s="111" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="113"/>
+      <c r="B12" s="111"/>
       <c r="C12" s="12" t="s">
         <v>32</v>
       </c>
@@ -5995,10 +6295,10 @@
       <c r="D18" s="11"/>
     </row>
     <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="113" t="s">
+      <c r="A19" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="113"/>
+      <c r="B19" s="111"/>
       <c r="C19" s="10" t="s">
         <v>18</v>
       </c>
@@ -6047,10 +6347,10 @@
       <c r="D24" s="12"/>
     </row>
     <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="113" t="s">
+      <c r="A25" s="111" t="s">
         <v>86</v>
       </c>
-      <c r="B25" s="113"/>
+      <c r="B25" s="111"/>
       <c r="C25" s="10" t="s">
         <v>51</v>
       </c>
@@ -6097,10 +6397,10 @@
       <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="113" t="s">
+      <c r="A30" s="111" t="s">
         <v>93</v>
       </c>
-      <c r="B30" s="113"/>
+      <c r="B30" s="111"/>
       <c r="C30" s="12" t="s">
         <v>60</v>
       </c>

</xml_diff>